<commit_message>
Change sample excel file
</commit_message>
<xml_diff>
--- a/WebContent/resources/sample.xlsx
+++ b/WebContent/resources/sample.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\glassfish4\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14895" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,34 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="11">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">Username </t>
   </si>
@@ -63,8 +32,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -92,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,109 +355,25 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>